<commit_message>
+= update vat invoice template
</commit_message>
<xml_diff>
--- a/WebAPI/eFMS.API.SystemWeb/eFMS.API.Accounting/eFMS.API.Accounting/Resources/Files/VatInvoiceImportTemplate.xlsx
+++ b/WebAPI/eFMS.API.SystemWeb/eFMS.API.Accounting/eFMS.API.Accounting/Resources/Files/VatInvoiceImportTemplate.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis.quang\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kenny.thuong\Desktop\eFms\WebAPI\eFMS.API.SystemWeb\eFMS.API.Accounting\eFMS.API.Accounting\Resources\Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -101,12 +101,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Alex Phuong:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Trạng thái thanh toán: Paid/Unpaid
+</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Real Invoice</t>
   </si>
@@ -119,11 +144,14 @@
   <si>
     <t>Voucher ID *</t>
   </si>
+  <si>
+    <t>Payment Status</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -476,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -488,9 +516,10 @@
     <col min="2" max="2" width="19.42578125" style="5" customWidth="1"/>
     <col min="3" max="3" width="14.140625" style="5" customWidth="1"/>
     <col min="4" max="4" width="9.140625" style="5"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -503,12 +532,16 @@
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="E1" s="3" t="s">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>